<commit_message>
Revert "Merge branch 'main' of https://github.com/Victorschimmell/SpiludviklingsProjekt into main"
This reverts commit a734268fdc3592783ea305a3980174d9360f7d68, reversing
changes made to 55a08f7da47681b5349cbc30726efa35f0b8c4ea.
</commit_message>
<xml_diff>
--- a/Burn-down-chart.xlsx
+++ b/Burn-down-chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardrostomian/Documents/GitHub/SpiludviklingsProjekt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\Github\SpiludviklingsProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8632FE6A-18E4-6B47-8046-6E7E046217CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2396D1-DAA1-4CE6-A3A2-7CC2DBB88B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -5742,67 +5742,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Billede 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0AF16CD-52E7-0A4C-A30E-3CC42A45716C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9474200" y="1524000"/>
-          <a:ext cx="7645400" cy="4127500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6071,16 +6010,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ES4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="77" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6676,7 +6615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6693,7 +6632,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7271,7 +7210,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:149" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>148</v>
       </c>

</xml_diff>